<commit_message>
Update algorithm, processing, and analysis
</commit_message>
<xml_diff>
--- a/variable/pe_social_contact_parameters.xlsx
+++ b/variable/pe_social_contact_parameters.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M38"/>
+  <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,19 +486,39 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Lower bound</t>
+          <t>Estimate lower bound</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Upper bound</t>
+          <t>Estimate upper bound</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Initial guess lower bound</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Initial guess upper bound</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Constraints lower bound</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Constraints upper bound</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Household contact probability</t>
+          <t>Probability of contact within household layer</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -532,16 +552,28 @@
         <v>0.9815642</v>
       </c>
       <c r="L2" t="n">
+        <v>0.9813744</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.9816373</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.9514584</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.9997778</v>
+      </c>
+      <c r="P2" t="n">
         <v>0.95</v>
       </c>
-      <c r="M2" t="n">
+      <c r="Q2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Household consecutive daily contact probability</t>
+          <t>Consecutive daily contact probability within household layer</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -575,16 +607,28 @@
         <v>0.406743</v>
       </c>
       <c r="L3" t="n">
+        <v>0.4035243</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.406743</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.4018447</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.9878015</v>
+      </c>
+      <c r="P3" t="n">
         <v>0.4</v>
       </c>
-      <c r="M3" t="n">
+      <c r="Q3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Household contact probability when health</t>
+          <t>Contact probability when healthy within household layer</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -618,16 +662,28 @@
         <v>0.0563526</v>
       </c>
       <c r="L4" t="n">
+        <v>0.0549288</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.057753</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.0519458</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.4999198</v>
+      </c>
+      <c r="P4" t="n">
         <v>0.05</v>
       </c>
-      <c r="M4" t="n">
+      <c r="Q4" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Household contact probability when symptomatic</t>
+          <t>Contact probability when symptomatic within household layer</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -661,16 +717,28 @@
         <v>0.0212009</v>
       </c>
       <c r="L5" t="n">
+        <v>0.0212009</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.0216763</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.0108859</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.0994009</v>
+      </c>
+      <c r="P5" t="n">
         <v>0.01</v>
       </c>
-      <c r="M5" t="n">
+      <c r="Q5" t="n">
         <v>0.1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Household steepness</t>
+          <t>Steepness of the logistic contact probability function within household layer</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -704,16 +772,28 @@
         <v>3.8905682</v>
       </c>
       <c r="L6" t="n">
+        <v>3.7553894</v>
+      </c>
+      <c r="M6" t="n">
+        <v>3.8905682</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1.2364132</v>
+      </c>
+      <c r="O6" t="n">
+        <v>19.9753985</v>
+      </c>
+      <c r="P6" t="n">
         <v>1</v>
       </c>
-      <c r="M6" t="n">
+      <c r="Q6" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Household phase relative to symptom-onset for symptomatic</t>
+          <t>Phase relative to symptom onset for symptomatic (days) within household layer</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -747,16 +827,28 @@
         <v>4.7717213</v>
       </c>
       <c r="L7" t="n">
+        <v>4.6765422</v>
+      </c>
+      <c r="M7" t="n">
+        <v>4.7717213</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.0986915</v>
+      </c>
+      <c r="O7" t="n">
+        <v>9.9010677</v>
+      </c>
+      <c r="P7" t="n">
         <v>0</v>
       </c>
-      <c r="M7" t="n">
+      <c r="Q7" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Household phase relative to symptomatic for resuming normal social context</t>
+          <t>Phase relative to symptom onset for resuming normal social context (days) within household layer</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -790,16 +882,28 @@
         <v>7.132223</v>
       </c>
       <c r="L8" t="n">
+        <v>7.1105597</v>
+      </c>
+      <c r="M8" t="n">
+        <v>7.1653285</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.0678561</v>
+      </c>
+      <c r="O8" t="n">
+        <v>9.841184200000001</v>
+      </c>
+      <c r="P8" t="n">
         <v>0</v>
       </c>
-      <c r="M8" t="n">
+      <c r="Q8" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>School contact probability</t>
+          <t>Probability of contact within school layer</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -833,16 +937,28 @@
         <v>0.8011814</v>
       </c>
       <c r="L9" t="n">
+        <v>0.8011814</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.8064416</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.1137086</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.9714956</v>
+      </c>
+      <c r="P9" t="n">
         <v>0.1</v>
       </c>
-      <c r="M9" t="n">
+      <c r="Q9" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>School consecutive daily contact probability</t>
+          <t>Consecutive daily contact probability within school layer</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -876,16 +992,28 @@
         <v>0.9074275000000001</v>
       </c>
       <c r="L10" t="n">
+        <v>0.9074275000000001</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.9098335</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.5020798</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.9911082</v>
+      </c>
+      <c r="P10" t="n">
         <v>0.5</v>
       </c>
-      <c r="M10" t="n">
+      <c r="Q10" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>School contact probability when health</t>
+          <t>Contact probability when healthy within school layer</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -919,16 +1047,28 @@
         <v>0.0135561</v>
       </c>
       <c r="L11" t="n">
+        <v>0.0127297</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.0158094</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.0109628</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.4999261</v>
+      </c>
+      <c r="P11" t="n">
         <v>0.01</v>
       </c>
-      <c r="M11" t="n">
+      <c r="Q11" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>School contact probability when symptomatic</t>
+          <t>Contact probability when symptomatic within school layer</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -962,16 +1102,28 @@
         <v>0.0431357</v>
       </c>
       <c r="L12" t="n">
+        <v>0.0429207</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.0432555</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.0018008</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.0490501</v>
+      </c>
+      <c r="P12" t="n">
         <v>0.001</v>
       </c>
-      <c r="M12" t="n">
+      <c r="Q12" t="n">
         <v>0.05</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>School steepness</t>
+          <t>Steepness of the logistic contact probability function within school layer</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -1005,16 +1157,28 @@
         <v>6.7182169</v>
       </c>
       <c r="L13" t="n">
+        <v>6.7171996</v>
+      </c>
+      <c r="M13" t="n">
+        <v>6.7834145</v>
+      </c>
+      <c r="N13" t="n">
+        <v>1.0637532</v>
+      </c>
+      <c r="O13" t="n">
+        <v>9.445391300000001</v>
+      </c>
+      <c r="P13" t="n">
         <v>1</v>
       </c>
-      <c r="M13" t="n">
+      <c r="Q13" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>School phase relative to symptom-onset for symptomatic</t>
+          <t>Phase relative to symptom onset for symptomatic (days) within school layer</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -1048,16 +1212,28 @@
         <v>9.9340981</v>
       </c>
       <c r="L14" t="n">
-        <v>0</v>
+        <v>9.9340981</v>
       </c>
       <c r="M14" t="n">
         <v>10</v>
       </c>
+      <c r="N14" t="n">
+        <v>0.1014381</v>
+      </c>
+      <c r="O14" t="n">
+        <v>9.9581626</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>School phase relative to symptomatic for resuming normal social context</t>
+          <t>Phase relative to symptom onset for resuming normal social context (days) within school layer</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -1091,16 +1267,28 @@
         <v>1.7266511</v>
       </c>
       <c r="L15" t="n">
+        <v>1.7065511</v>
+      </c>
+      <c r="M15" t="n">
+        <v>1.7727431</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.0041295</v>
+      </c>
+      <c r="O15" t="n">
+        <v>9.8999123</v>
+      </c>
+      <c r="P15" t="n">
         <v>0</v>
       </c>
-      <c r="M15" t="n">
+      <c r="Q15" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>Workplace contact probability</t>
+          <t>Probability of contact within workplace layer</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -1134,16 +1322,28 @@
         <v>0.2188239</v>
       </c>
       <c r="L16" t="n">
+        <v>0.2141153</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.2188239</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.1010826</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.9967066</v>
+      </c>
+      <c r="P16" t="n">
         <v>0.1</v>
       </c>
-      <c r="M16" t="n">
+      <c r="Q16" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>Workplace consecutive daily contact probability</t>
+          <t>Consecutive daily contact probability within workplace layer</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -1177,16 +1377,28 @@
         <v>0.5655395</v>
       </c>
       <c r="L17" t="n">
+        <v>0.5632769</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.5669683</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.5039645</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.9994351</v>
+      </c>
+      <c r="P17" t="n">
         <v>0.5</v>
       </c>
-      <c r="M17" t="n">
+      <c r="Q17" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Workplace contact probability when health</t>
+          <t>Contact probability when healthy within workplace layer</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -1220,16 +1432,28 @@
         <v>0.0355397</v>
       </c>
       <c r="L18" t="n">
+        <v>0.0355397</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.0380466</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.0122231</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.4913164</v>
+      </c>
+      <c r="P18" t="n">
         <v>0.01</v>
       </c>
-      <c r="M18" t="n">
+      <c r="Q18" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Workplace contact probability when symptomatic</t>
+          <t>Contact probability when symptomatic within workplace layer</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -1263,16 +1487,28 @@
         <v>0.0206327</v>
       </c>
       <c r="L19" t="n">
+        <v>0.0201447</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.0206327</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.002221</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0.049448</v>
+      </c>
+      <c r="P19" t="n">
         <v>0.001</v>
       </c>
-      <c r="M19" t="n">
+      <c r="Q19" t="n">
         <v>0.05</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Workplace steepness</t>
+          <t>Steepness of the logistic contact probability function within workplace layer</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -1306,16 +1542,28 @@
         <v>2.7870861</v>
       </c>
       <c r="L20" t="n">
+        <v>2.7617305</v>
+      </c>
+      <c r="M20" t="n">
+        <v>2.8686074</v>
+      </c>
+      <c r="N20" t="n">
+        <v>1.072661</v>
+      </c>
+      <c r="O20" t="n">
+        <v>9.7834415</v>
+      </c>
+      <c r="P20" t="n">
         <v>1</v>
       </c>
-      <c r="M20" t="n">
+      <c r="Q20" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Workplace phase relative to symptom-onset for symptomatic</t>
+          <t>Phase relative to symptom onset for symptomatic (days) within workplace layer</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -1349,16 +1597,28 @@
         <v>2.6870014</v>
       </c>
       <c r="L21" t="n">
+        <v>2.6870014</v>
+      </c>
+      <c r="M21" t="n">
+        <v>2.7917888</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0.0046317</v>
+      </c>
+      <c r="O21" t="n">
+        <v>9.996922100000001</v>
+      </c>
+      <c r="P21" t="n">
         <v>0</v>
       </c>
-      <c r="M21" t="n">
+      <c r="Q21" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>Workplace phase relative to symptomatic for resuming normal social context</t>
+          <t>Phase relative to symptom onset for resuming normal social context (days) within workplace layer</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -1392,16 +1652,28 @@
         <v>6.8444106</v>
       </c>
       <c r="L22" t="n">
+        <v>6.8170766</v>
+      </c>
+      <c r="M22" t="n">
+        <v>6.8714812</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0.0332962</v>
+      </c>
+      <c r="O22" t="n">
+        <v>9.844794200000001</v>
+      </c>
+      <c r="P22" t="n">
         <v>0</v>
       </c>
-      <c r="M22" t="n">
+      <c r="Q22" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Heath care contact probability</t>
+          <t>Probability of contact within heath care layer</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -1435,16 +1707,28 @@
         <v>0.0060079</v>
       </c>
       <c r="L23" t="n">
+        <v>0.0059791</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0.0060079</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0.005001</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0.0079966</v>
+      </c>
+      <c r="P23" t="n">
         <v>0.005</v>
       </c>
-      <c r="M23" t="n">
+      <c r="Q23" t="n">
         <v>0.008</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Heath care consecutive daily contact probability</t>
+          <t>Consecutive daily contact probability within heath care layer</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -1478,16 +1762,28 @@
         <v>0.84502</v>
       </c>
       <c r="L24" t="n">
+        <v>0.8415189</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.8473494</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0.5064355</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0.9935533</v>
+      </c>
+      <c r="P24" t="n">
         <v>0.5</v>
       </c>
-      <c r="M24" t="n">
+      <c r="Q24" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Heath care contact probability when health</t>
+          <t>Contact probability when healthy within heath care layer</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -1521,16 +1817,28 @@
         <v>0.002285</v>
       </c>
       <c r="L25" t="n">
+        <v>0.0022543</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.0023189</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0.0010241</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0.0059853</v>
+      </c>
+      <c r="P25" t="n">
         <v>0.001</v>
       </c>
-      <c r="M25" t="n">
+      <c r="Q25" t="n">
         <v>0.006</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Heath care contact probability when symptomatic</t>
+          <t>Contact probability when symptomatic within heath care layer</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -1564,16 +1872,28 @@
         <v>0.719144</v>
       </c>
       <c r="L26" t="n">
+        <v>0.7168134</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.719144</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0.6049105</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0.9980445</v>
+      </c>
+      <c r="P26" t="n">
         <v>0.6</v>
       </c>
-      <c r="M26" t="n">
+      <c r="Q26" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Heath care steepness</t>
+          <t>Steepness of the logistic contact probability function within heath care layer</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -1607,16 +1927,28 @@
         <v>4.2179046</v>
       </c>
       <c r="L27" t="n">
+        <v>4.1730533</v>
+      </c>
+      <c r="M27" t="n">
+        <v>4.225386</v>
+      </c>
+      <c r="N27" t="n">
+        <v>1.1089668</v>
+      </c>
+      <c r="O27" t="n">
+        <v>9.916226399999999</v>
+      </c>
+      <c r="P27" t="n">
         <v>1</v>
       </c>
-      <c r="M27" t="n">
+      <c r="Q27" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Heath care phase relative to symptom-onset for symptomatic</t>
+          <t>Phase relative to symptom onset for symptomatic (days) within heath care layer</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -1650,16 +1982,28 @@
         <v>9.345397</v>
       </c>
       <c r="L28" t="n">
+        <v>9.345397</v>
+      </c>
+      <c r="M28" t="n">
+        <v>9.3850803</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0.0174672</v>
+      </c>
+      <c r="O28" t="n">
+        <v>9.9391382</v>
+      </c>
+      <c r="P28" t="n">
         <v>0</v>
       </c>
-      <c r="M28" t="n">
+      <c r="Q28" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>Heath care phase relative to symptomatic for resuming normal social context</t>
+          <t>Phase relative to symptom onset for resuming normal social context (days) within heath care layer</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -1693,16 +2037,28 @@
         <v>4.4248827</v>
       </c>
       <c r="L29" t="n">
+        <v>4.3731756</v>
+      </c>
+      <c r="M29" t="n">
+        <v>4.438816</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0.1601804</v>
+      </c>
+      <c r="O29" t="n">
+        <v>9.9270844</v>
+      </c>
+      <c r="P29" t="n">
         <v>0</v>
       </c>
-      <c r="M29" t="n">
+      <c r="Q29" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>Municipality contact probability</t>
+          <t>Probability of contact within municipality layer</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -1736,16 +2092,28 @@
         <v>7.4e-06</v>
       </c>
       <c r="L30" t="n">
+        <v>7.4e-06</v>
+      </c>
+      <c r="M30" t="n">
+        <v>7.4e-06</v>
+      </c>
+      <c r="N30" t="n">
+        <v>2.1e-06</v>
+      </c>
+      <c r="O30" t="n">
+        <v>9.9e-06</v>
+      </c>
+      <c r="P30" t="n">
         <v>2e-06</v>
       </c>
-      <c r="M30" t="n">
+      <c r="Q30" t="n">
         <v>1e-05</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>Municipality consecutive daily contact probability</t>
+          <t>Consecutive daily contact probability within municipality layer</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -1779,16 +2147,28 @@
         <v>0.5709235</v>
       </c>
       <c r="L31" t="n">
+        <v>0.5677729</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0.5725763</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0.5081613</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0.995623</v>
+      </c>
+      <c r="P31" t="n">
         <v>0.5</v>
       </c>
-      <c r="M31" t="n">
+      <c r="Q31" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>Municipality contact probability when health</t>
+          <t>Contact probability when healthy within municipality layer</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -1822,16 +2202,28 @@
         <v>0.010782</v>
       </c>
       <c r="L32" t="n">
+        <v>0.01047</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0.0108936</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0.010305</v>
+      </c>
+      <c r="O32" t="n">
+        <v>0.0997263</v>
+      </c>
+      <c r="P32" t="n">
         <v>0.01</v>
       </c>
-      <c r="M32" t="n">
+      <c r="Q32" t="n">
         <v>0.1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Municipality contact probability when symptomatic</t>
+          <t>Contact probability when symptomatic within municipality layer</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -1865,16 +2257,28 @@
         <v>0.0492931</v>
       </c>
       <c r="L33" t="n">
+        <v>0.048963</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0.0494151</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0.0011979</v>
+      </c>
+      <c r="O33" t="n">
+        <v>0.0499194</v>
+      </c>
+      <c r="P33" t="n">
         <v>0.001</v>
       </c>
-      <c r="M33" t="n">
+      <c r="Q33" t="n">
         <v>0.05</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>Municipality steepness</t>
+          <t>Steepness of the logistic contact probability function within municipality layer</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -1908,16 +2312,28 @@
         <v>3.3402714</v>
       </c>
       <c r="L34" t="n">
+        <v>3.3325891</v>
+      </c>
+      <c r="M34" t="n">
+        <v>3.400308</v>
+      </c>
+      <c r="N34" t="n">
+        <v>1.1983502</v>
+      </c>
+      <c r="O34" t="n">
+        <v>9.8401297</v>
+      </c>
+      <c r="P34" t="n">
         <v>1</v>
       </c>
-      <c r="M34" t="n">
+      <c r="Q34" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Municipality phase relative to symptom-onset for symptomatic</t>
+          <t>Phase relative to symptom onset for symptomatic (days) within municipality layer</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1951,16 +2367,28 @@
         <v>7.3818604</v>
       </c>
       <c r="L35" t="n">
+        <v>7.33048</v>
+      </c>
+      <c r="M35" t="n">
+        <v>7.4362635</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0.1208321</v>
+      </c>
+      <c r="O35" t="n">
+        <v>9.765071600000001</v>
+      </c>
+      <c r="P35" t="n">
         <v>0</v>
       </c>
-      <c r="M35" t="n">
+      <c r="Q35" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>Municipality phase relative to symptomatic for resuming normal social context</t>
+          <t>Phase relative to symptom onset for resuming normal social context (days) within municipality layer</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1994,16 +2422,28 @@
         <v>9.9477663</v>
       </c>
       <c r="L36" t="n">
+        <v>9.891370200000001</v>
+      </c>
+      <c r="M36" t="n">
+        <v>9.9477663</v>
+      </c>
+      <c r="N36" t="n">
+        <v>0.0159508</v>
+      </c>
+      <c r="O36" t="n">
+        <v>9.9239655</v>
+      </c>
+      <c r="P36" t="n">
         <v>0</v>
       </c>
-      <c r="M36" t="n">
+      <c r="Q36" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>overdispersion rate</t>
+          <t>Overdispersion rate</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -2037,16 +2477,28 @@
         <v>0.1671147</v>
       </c>
       <c r="L37" t="n">
+        <v>0.166497</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0.1679448</v>
+      </c>
+      <c r="N37" t="n">
+        <v>0.0025337</v>
+      </c>
+      <c r="O37" t="n">
+        <v>0.19394</v>
+      </c>
+      <c r="P37" t="n">
         <v>0</v>
       </c>
-      <c r="M37" t="n">
+      <c r="Q37" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>overdispersion weight</t>
+          <t>Overdispersion weight</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -2080,9 +2532,21 @@
         <v>6.308076</v>
       </c>
       <c r="L38" t="n">
+        <v>6.2801237</v>
+      </c>
+      <c r="M38" t="n">
+        <v>6.4135898</v>
+      </c>
+      <c r="N38" t="n">
+        <v>1.1236438</v>
+      </c>
+      <c r="O38" t="n">
+        <v>19.3580253</v>
+      </c>
+      <c r="P38" t="n">
         <v>1</v>
       </c>
-      <c r="M38" t="n">
+      <c r="Q38" t="n">
         <v>20</v>
       </c>
     </row>

</xml_diff>